<commit_message>
Thêm câu hỏi vào ngân hàng đề NMCNTT chương 4
</commit_message>
<xml_diff>
--- a/Nhập môn Công nghệ thông tin/deCNTT1116_C4.xlsx
+++ b/Nhập môn Công nghệ thông tin/deCNTT1116_C4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Phát triển đề SITDE PK\SITDE-PK-BANKS\Nhập môn Công nghệ thông tin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6BB26D3-F08B-45A4-85EE-DDB5BDEC6E49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9BC37B7-59CC-49EB-B464-476295216D4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="326">
   <si>
     <t>Cho biểu thức A= (-3+4%5/2) Giá trị của biểu thức A là:</t>
   </si>
@@ -946,10 +946,251 @@
     <t>Lỗi chương trình</t>
   </si>
   <si>
+    <t>10</t>
+  </si>
+  <si>
     <t>Phát biểu nào sau đây SAI về vòng lặp for?</t>
   </si>
   <si>
     <t>Câu này không có giải thích.</t>
+  </si>
+  <si>
+    <t>Hãy cho biết kết quả khi chạy chương trình:
+int y = 128;
+const int x = 128;
+x = --y;
+printf("%d\n", x);</t>
+  </si>
+  <si>
+    <t>128</t>
+  </si>
+  <si>
+    <t>127</t>
+  </si>
+  <si>
+    <t>-127</t>
+  </si>
+  <si>
+    <t>Một thông báo lỗi</t>
+  </si>
+  <si>
+    <t>Biến x được khai báo là hằng số, nên không thể gán được giá trị khác cho x.</t>
+  </si>
+  <si>
+    <t>Hãy cho biết kết quả của đoạn lệnh sau:
+#include &lt;stdio.h&gt;
+void main()
+{
+    int x = 10, y = 20, z = 5, i;
+    i = x &lt; y &lt; z;
+    printf("%d\n", i);
+}</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>Phép toán so sánh được thực hiện từ trái qua phải. Vậy nên, trong phép toán x &lt; y &lt; z, trước hết ta thực hiện so sánh x và y. Vì x = 10 và y = 20, nên phép toán x &lt; y có giá trị đúng và trả về kết quả 1. Sau đó, ta so sánh x &lt; y với z, hay nói cách khác, ta so sánh 1 với z = 5. Vì 1 &lt; 5 là đúng nên phép toán trả về kết quả 1.</t>
+  </si>
+  <si>
+    <t>Chọn khẳng định ĐÚNG trong các khẳng định dưới đây:</t>
+  </si>
+  <si>
+    <t>Các phần tử (hay biến) trong mảng một chiều có cùng kiểu dữ liệu.</t>
+  </si>
+  <si>
+    <t>Các phần tử (hay biến) trong mảng một chiều có thể khác kiểu dữ liệu.</t>
+  </si>
+  <si>
+    <t>Vòng lặp while là lựa chọn lý tưởng để thao tác với các mảng.</t>
+  </si>
+  <si>
+    <t>Vòng lặp do…while là lựa chọn lý tưởng để thao tác với các mảng.</t>
+  </si>
+  <si>
+    <t>- Mảng (Array) một chiều là tập hợp các phần tử (hay biến) cùng kiểu dữ liệu, cùng tên và được cấp phát các vùng nhớ liên tiếp nhau trong bộ nhớ.
+- Vòng lặp for là lựa chọn lý tưởng để thao tác với các mảng.</t>
+  </si>
+  <si>
+    <t>Đâu là cách khai báo mảng đúng?</t>
+  </si>
+  <si>
+    <t>int a(10)</t>
+  </si>
+  <si>
+    <t>float b[50]</t>
+  </si>
+  <si>
+    <t>char ht{25}[23]</t>
+  </si>
+  <si>
+    <t>double c[12]{7}</t>
+  </si>
+  <si>
+    <t>Với khai báo int toado[10][20] thì mảng toado có bao nhiêu phần tử?</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>Điền vào chỗ trống để hoàn thành chương trình tìm số lớn nhất giữa 2 số?
+#include &lt;stdio.h&gt;
+void main()
+{
+    int a, b, max;
+    printf("Nhap gia tri cua a va b: ");
+    scanf("%d %d", &amp;a, &amp;b);
+    if (............)
+        max = a;
+    else
+        max = b;
+    printf("So lon nhat trong 2 so %d va %d la %d", a, b, max);
+}</t>
+  </si>
+  <si>
+    <t>a&gt;b</t>
+  </si>
+  <si>
+    <t>a&lt;b</t>
+  </si>
+  <si>
+    <t>a=b</t>
+  </si>
+  <si>
+    <t>a!=b</t>
+  </si>
+  <si>
+    <t>Cho biết kết quả in ra màn hình: printf("%d", 0.1 == 0.1f);</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>Kết quả in ra màn hình của chương trình sau:
+#include &lt;stdio.h&gt;
+void main()
+{
+    int i=5, j=6;
+    i = i - --j;
+    printf("%d", i);
+}</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Trong C, đoạn mã sau hiển thị gì trên màn hình?
+#include &lt;stdio.h&gt;
+void main()
+{
+    int i = 0;
+    while (++i+1&lt;=5)
+        printf("%d", i);
+}</t>
+  </si>
+  <si>
+    <t>12345</t>
+  </si>
+  <si>
+    <t>01234</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>Cho biết kết quả hiển thị trên màn hình?
+   int a;
+   for (a=1; a&lt;=10; a++){
+       printf("%i ",a);
+       if (a%3)
+        a = a + 2;
+   }</t>
+  </si>
+  <si>
+    <t>1 4 7</t>
+  </si>
+  <si>
+    <t>1 3 5 7 9</t>
+  </si>
+  <si>
+    <t>1 4 7 10</t>
+  </si>
+  <si>
+    <t>1 4 8</t>
+  </si>
+  <si>
+    <t>Hãy cho biết kết quả khi chạy chương trình: 
+#include &lt;stdio.h&gt;
+#define a 10
+int main()
+{
+    printf("%d ", a);
+    #define a 50
+    printf("%d ", a);
+    return 0;
+}</t>
+  </si>
+  <si>
+    <t>10 50</t>
+  </si>
+  <si>
+    <t>Lỗi biên dịch</t>
+  </si>
+  <si>
+    <t>10 10</t>
+  </si>
+  <si>
+    <t>50 50</t>
+  </si>
+  <si>
+    <t>Tìm lỗi sai trong chương trình sau (in ra kết quả là tổng của 123 và 456):
+#include &lt;stdio.h&gt;
+void main()
+{
+    int sum;
+    sum = 453 + 343
+    printf("\Ket qua la: ", sum);
+}</t>
+  </si>
+  <si>
+    <t>Thiếu dấu chấm phẩy</t>
+  </si>
+  <si>
+    <t>Thiếu dấu phẩy</t>
+  </si>
+  <si>
+    <t>Thiếu mã định dạng</t>
+  </si>
+  <si>
+    <t>Kết quả chương trình C sau là gì?
+#include &lt;stdio.h&gt;
+int main()
+{
+    int xyz = 20;
+    {
+        int xyz = 40;
+    }
+    printf("%d", xyz);
+    return 0;
+}</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>Vì lệnh printf ở cùng khối lệnh với biến xyz toàn cục, nên kết quả hiển thị ra màn hình sẽ là giá trị của biến toàn cục xyz = 20, chứ không phải của biến cục bộ xyz = 40 (nằm ở khối lệnh bên trong cùng).</t>
   </si>
 </sst>
 </file>
@@ -1282,10 +1523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G64"/>
+  <dimension ref="A1:G77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G65" sqref="G65"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1317,7 +1558,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1340,7 +1581,7 @@
         <v>4</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="105" x14ac:dyDescent="0.25">
@@ -1455,7 +1696,7 @@
         <v>4</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1478,7 +1719,7 @@
         <v>10</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1501,7 +1742,7 @@
         <v>10</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -1524,7 +1765,7 @@
         <v>38</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1547,7 +1788,7 @@
         <v>38</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="225" x14ac:dyDescent="0.25">
@@ -1593,7 +1834,7 @@
         <v>4</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -1662,7 +1903,7 @@
         <v>10</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1685,7 +1926,7 @@
         <v>4</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -1731,7 +1972,7 @@
         <v>4</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="120" x14ac:dyDescent="0.25">
@@ -1754,7 +1995,7 @@
         <v>38</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -1777,7 +2018,7 @@
         <v>4</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="150" x14ac:dyDescent="0.25">
@@ -1800,7 +2041,7 @@
         <v>10</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="150" x14ac:dyDescent="0.25">
@@ -1823,7 +2064,7 @@
         <v>4</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="150" x14ac:dyDescent="0.25">
@@ -1846,7 +2087,7 @@
         <v>38</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="150" x14ac:dyDescent="0.25">
@@ -1869,7 +2110,7 @@
         <v>3</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1892,7 +2133,7 @@
         <v>3</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1915,7 +2156,7 @@
         <v>10</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -1938,7 +2179,7 @@
         <v>4</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="150" x14ac:dyDescent="0.25">
@@ -1961,7 +2202,7 @@
         <v>10</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="150" x14ac:dyDescent="0.25">
@@ -1984,7 +2225,7 @@
         <v>4</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="135" x14ac:dyDescent="0.25">
@@ -2007,7 +2248,7 @@
         <v>10</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="90" x14ac:dyDescent="0.25">
@@ -2030,7 +2271,7 @@
         <v>38</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -2053,7 +2294,7 @@
         <v>4</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2076,7 +2317,7 @@
         <v>10</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2099,7 +2340,7 @@
         <v>10</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -2122,7 +2363,7 @@
         <v>3</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="150" x14ac:dyDescent="0.25">
@@ -2145,7 +2386,7 @@
         <v>38</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2168,7 +2409,7 @@
         <v>3</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -2191,7 +2432,7 @@
         <v>3</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -2214,7 +2455,7 @@
         <v>4</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2237,10 +2478,10 @@
         <v>38</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>170</v>
       </c>
@@ -2260,7 +2501,7 @@
         <v>4</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -2283,7 +2524,7 @@
         <v>10</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -2306,7 +2547,7 @@
         <v>3</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -2329,7 +2570,7 @@
         <v>4</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -2352,7 +2593,7 @@
         <v>4</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="135" x14ac:dyDescent="0.25">
@@ -2375,7 +2616,7 @@
         <v>38</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="135" x14ac:dyDescent="0.25">
@@ -2398,12 +2639,12 @@
         <v>4</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>200</v>
@@ -2421,7 +2662,7 @@
         <v>38</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2444,7 +2685,7 @@
         <v>38</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2467,7 +2708,7 @@
         <v>3</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -2490,7 +2731,7 @@
         <v>38</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="165" x14ac:dyDescent="0.25">
@@ -2513,7 +2754,7 @@
         <v>4</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="195" x14ac:dyDescent="0.25">
@@ -2536,7 +2777,7 @@
         <v>38</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="135" x14ac:dyDescent="0.25">
@@ -2559,7 +2800,7 @@
         <v>4</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="165" x14ac:dyDescent="0.25">
@@ -2582,7 +2823,7 @@
         <v>38</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="210" x14ac:dyDescent="0.25">
@@ -2720,7 +2961,7 @@
         <v>10</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="135" x14ac:dyDescent="0.25">
@@ -2743,7 +2984,7 @@
         <v>4</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="165" x14ac:dyDescent="0.25">
@@ -2766,7 +3007,306 @@
         <v>38</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="210" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="285" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G74" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="180" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="165" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>325</v>
       </c>
     </row>
   </sheetData>

</xml_diff>